<commit_message>
Se crea el primer archivo .rkt y se agregan funciones auxiliares
Se agregan las funciones:
-tamano-lista
-miembro?
-eliminar
</commit_message>
<xml_diff>
--- a/Plan de Actividades.xlsx
+++ b/Plan de Actividades.xlsx
@@ -1,26 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\2021_LENGUAJES_TAREA_1_BLACEJACK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC122CF4-A068-4D9F-88B1-234F91690D7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9C3F908-519C-42D8-BB57-E53B170551D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Responsable a cargo</t>
+  </si>
+  <si>
+    <t>Tiempo estimado de completitud</t>
+  </si>
+  <si>
+    <t>Descripción de la tarea</t>
+  </si>
+  <si>
+    <t>Fecha de entrega</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +63,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +93,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,7 +134,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -85,7 +150,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +162,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -114,7 +179,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -144,12 +209,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -179,6 +261,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +429,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FABEE4C-4A90-408D-BADB-43F9A07AF694}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.21875" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>